<commit_message>
Rental Manager Functions Completed
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/Team_2_Iteration 2_Submission/Previously submitted Files/UCID Table (Updated).xlsx
+++ b/Iteration 2 docs/Team_2_Iteration 2_Submission/Previously submitted Files/UCID Table (Updated).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS 2020\ArlingtonAuto\Iteration 2 docs\Team_2_Iteration 2\Previously submitted Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sem3\SE\ArlingtonAuto\Iteration 2 docs\Team_2_Iteration 2_Submission\Previously submitted Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009D0302-5DB6-4383-85B0-DFD17F6A4711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0D4D64-25F2-4E56-80EA-5B2BC613F908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={72E90268-882F-4B09-B67C-29CA277D1BA0}</author>
+    <author>tc={50C6910E-A1B8-40D5-A781-EA0F6464BFB0}</author>
+    <author>tc={417185B6-E429-4068-85B5-8169B33866DD}</author>
   </authors>
   <commentList>
     <comment ref="B16" authorId="0" shapeId="0" xr:uid="{72E90268-882F-4B09-B67C-29CA277D1BA0}">
@@ -47,6 +49,22 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Changed Edit User Profile to Modify User Profile</t>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="1" shapeId="0" xr:uid="{50C6910E-A1B8-40D5-A781-EA0F6464BFB0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    removing car number bc not stored in reservation table. Displaying occupant capacity instead of car occupant capacity</t>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="2" shapeId="0" xr:uid="{417185B6-E429-4068-85B5-8169B33866DD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    removing car number, lastname, club membership bc not stored in reservation table. Displaying occupant capacity instead of car occupant capacity</t>
       </text>
     </comment>
   </commentList>
@@ -541,16 +559,6 @@
 End Date (default=Today)</t>
   </si>
   <si>
-    <t>Car Number
-Car Name
-Car Occupant Capacity
-Start Date
-Start Time
-End Date
-End Time
-Total Cost</t>
-  </si>
-  <si>
     <t>View Reservation Calender Screen (Rental Manager can navigate back to homescreen)</t>
   </si>
   <si>
@@ -561,23 +569,6 @@
   </si>
   <si>
     <t>View Reservation Calender Screen</t>
-  </si>
-  <si>
-    <t>Reservation number
-Car Number
-Car Name
-Car Occupant Capacity
-Last Name 
-First Name
-Start Date
-Start Time
-End Date
-End Time
-Total cost
-Gps selected
-Sirius selected
-On star selected
-Club Membership status (User only)</t>
   </si>
   <si>
     <t>View Rental Details Screen (Rental Manager can navigate back to View Reservation Calender screen OR his homescreen)</t>
@@ -740,12 +731,114 @@
       <t>Car Status</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reservation number
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Car Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Car Name
+Car Occupant Capacity
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Last Name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+First Name
+Start Date
+Start Time
+End Date
+End Time
+Total cost
+Gps selected
+Sirius selected
+On star selected
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Club Membership status (User only)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Car Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Car Name
+Occupant Capacity
+Start Date
+Start Time
+End Date
+End Time
+Total Cost</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -906,6 +999,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1337,7 +1444,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1405,9 +1512,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1416,6 +1520,18 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1805,6 +1921,12 @@
   <threadedComment ref="B16" dT="2020-10-17T20:12:28.45" personId="{C553B8B3-CB95-4EA1-A3C6-D2417E2358A5}" id="{72E90268-882F-4B09-B67C-29CA277D1BA0}">
     <text>Changed Edit User Profile to Modify User Profile</text>
   </threadedComment>
+  <threadedComment ref="F19" dT="2020-11-18T21:39:27.59" personId="{C553B8B3-CB95-4EA1-A3C6-D2417E2358A5}" id="{50C6910E-A1B8-40D5-A781-EA0F6464BFB0}">
+    <text>removing car number bc not stored in reservation table. Displaying occupant capacity instead of car occupant capacity</text>
+  </threadedComment>
+  <threadedComment ref="F20" dT="2020-11-18T21:40:09.96" personId="{C553B8B3-CB95-4EA1-A3C6-D2417E2358A5}" id="{417185B6-E429-4068-85B5-8169B33866DD}">
+    <text>removing car number, lastname, club membership bc not stored in reservation table. Displaying occupant capacity instead of car occupant capacity</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1812,24 +1934,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="29.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="29.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="43" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="3"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1855,7 +1977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1881,7 +2003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1907,7 +2029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1917,7 +2039,7 @@
       <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -1933,7 +2055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1959,7 +2081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1985,7 +2107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -2011,7 +2133,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -2037,7 +2159,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="145.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="145.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -2063,7 +2185,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2089,7 +2211,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2115,7 +2237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2141,7 +2263,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2167,7 +2289,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -2193,7 +2315,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -2219,7 +2341,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -2245,7 +2367,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>16</v>
       </c>
@@ -2271,7 +2393,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -2297,163 +2419,163 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+    <row r="19" spans="1:8" s="29" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="26">
         <v>16</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="H19" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>89</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D22" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="H22" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>20</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>109</v>
+      <c r="B23" s="25" t="s">
+        <v>107</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>89</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2463,7 +2585,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2473,7 +2595,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2506,89 +2628,89 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2602,7 +2724,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>